<commit_message>
Modelo corrigido e está rodando em 600Hz até 0.01s condições de contorno corretas e resultados animadores.
</commit_message>
<xml_diff>
--- a/LinerAxi_PT_155dB_1500Hz/Log/Log.xlsx
+++ b/LinerAxi_PT_155dB_1500Hz/Log/Log.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>================================================================================</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>Velocity field (comp1.u): 1</t>
+  </si>
+  <si>
+    <t>Não convergiu</t>
   </si>
 </sst>
 </file>
@@ -464,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A51"/>
+  <dimension ref="A1:A52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,7 +721,13 @@
         <v>40</v>
       </c>
     </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>